<commit_message>
Calculo da rentabilidade de dividendo para FII
</commit_message>
<xml_diff>
--- a/Planejamento Financeiro (1).xlsx
+++ b/Planejamento Financeiro (1).xlsx
@@ -2,19 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yukak\Documents\eclipse-workspace\wally\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0DF24B-B43D-4807-AFDF-4128C3E780F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843801FD-3521-4DA9-A600-CC3F4EAAB0B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24912" yWindow="744" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FII Compra" sheetId="5" r:id="rId1"/>
-    <sheet name="FII" sheetId="13" state="hidden" r:id="rId2"/>
+    <sheet name="Compra" sheetId="5" r:id="rId1"/>
+    <sheet name="Dividendo" sheetId="14" r:id="rId2"/>
+    <sheet name="FII" sheetId="13" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="26">
   <si>
     <t>Data</t>
   </si>
@@ -123,6 +124,24 @@
   <si>
     <t>-</t>
   </si>
+  <si>
+    <t>Cota</t>
+  </si>
+  <si>
+    <t>Dividendo/Cota</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>BBSE3</t>
+  </si>
+  <si>
+    <t>WIZ3</t>
+  </si>
+  <si>
+    <t>ALZR11</t>
+  </si>
 </sst>
 </file>
 
@@ -132,7 +151,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="d/mmm"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -205,6 +224,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -238,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -299,6 +332,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,7 +668,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Planilha1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:X986"/>
@@ -638,7 +676,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="C2" sqref="C2"/>
-      <selection pane="topRight" activeCell="C13" sqref="C13"/>
+      <selection pane="topRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -651,17 +689,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="38"/>
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="38" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="9"/>
@@ -698,7 +736,7 @@
         <v>102.36</v>
       </c>
       <c r="E2" s="14">
-        <f t="shared" ref="E2:E57" si="0">IF(A2="","",C2*D2)</f>
+        <f>IF(A2="","",C2*D2)</f>
         <v>204.72</v>
       </c>
       <c r="F2" s="15"/>
@@ -740,7 +778,7 @@
         <v>106.58</v>
       </c>
       <c r="E3" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A3="","",C3*D3)</f>
         <v>319.74</v>
       </c>
       <c r="F3" s="15"/>
@@ -782,7 +820,7 @@
         <v>106.03</v>
       </c>
       <c r="E4" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A4="","",C4*D4)</f>
         <v>106.03</v>
       </c>
       <c r="F4" s="15"/>
@@ -824,7 +862,7 @@
         <v>9.82</v>
       </c>
       <c r="E5" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A5="","",C5*D5)</f>
         <v>117.84</v>
       </c>
       <c r="F5" s="15"/>
@@ -866,7 +904,7 @@
         <v>105</v>
       </c>
       <c r="E6" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A6="","",C6*D6)</f>
         <v>210</v>
       </c>
       <c r="F6" s="15"/>
@@ -903,7 +941,7 @@
         <v>105.99</v>
       </c>
       <c r="E7" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A7="","",C7*D7)</f>
         <v>423.96</v>
       </c>
       <c r="F7" s="15"/>
@@ -935,7 +973,7 @@
         <v>102.35</v>
       </c>
       <c r="E8" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A8="","",C8*D8)</f>
         <v>409.4</v>
       </c>
       <c r="F8" s="18"/>
@@ -967,7 +1005,7 @@
         <v>106.3</v>
       </c>
       <c r="E9" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A9="","",C9*D9)</f>
         <v>212.6</v>
       </c>
       <c r="F9" s="18"/>
@@ -999,7 +1037,7 @@
         <v>126.75</v>
       </c>
       <c r="E10" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A10="","",C10*D10)</f>
         <v>380.25</v>
       </c>
       <c r="F10" s="18"/>
@@ -1028,7 +1066,7 @@
         <v>104.61</v>
       </c>
       <c r="E11" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A11="","",C11*D11)</f>
         <v>209.22</v>
       </c>
       <c r="F11" s="18"/>
@@ -1057,7 +1095,7 @@
         <v>77.5</v>
       </c>
       <c r="E12" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A12="","",C12*D12)</f>
         <v>310</v>
       </c>
       <c r="F12" s="18"/>
@@ -1086,7 +1124,7 @@
         <v>100.87</v>
       </c>
       <c r="E13" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A13="","",C13*D13)</f>
         <v>403.48</v>
       </c>
       <c r="F13" s="18"/>
@@ -1115,7 +1153,7 @@
         <v>126.3</v>
       </c>
       <c r="E14" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A14="","",C14*D14)</f>
         <v>252.6</v>
       </c>
       <c r="F14" s="18"/>
@@ -1144,7 +1182,7 @@
         <v>126.01</v>
       </c>
       <c r="E15" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A15="","",C15*D15)</f>
         <v>252.02</v>
       </c>
       <c r="F15" s="18"/>
@@ -1173,7 +1211,7 @@
         <v>100.15</v>
       </c>
       <c r="E16" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A16="","",C16*D16)</f>
         <v>200.3</v>
       </c>
       <c r="F16" s="18"/>
@@ -1202,7 +1240,7 @@
         <v>122.8</v>
       </c>
       <c r="E17" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A17="","",C17*D17)</f>
         <v>491.2</v>
       </c>
       <c r="F17" s="18"/>
@@ -1227,7 +1265,7 @@
         <v>97.85</v>
       </c>
       <c r="E18" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A18="","",C18*D18)</f>
         <v>489.25</v>
       </c>
       <c r="F18" s="18"/>
@@ -1252,7 +1290,7 @@
         <v>9.7799999999999994</v>
       </c>
       <c r="E19" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A19="","",C19*D19)</f>
         <v>97.8</v>
       </c>
       <c r="F19" s="18"/>
@@ -1277,7 +1315,7 @@
         <v>122.01</v>
       </c>
       <c r="E20" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A20="","",C20*D20)</f>
         <v>488.04</v>
       </c>
       <c r="F20" s="18"/>
@@ -1301,7 +1339,7 @@
         <v>97</v>
       </c>
       <c r="E21" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A21="","",C21*D21)</f>
         <v>388</v>
       </c>
       <c r="F21" s="18"/>
@@ -1325,7 +1363,7 @@
         <v>106</v>
       </c>
       <c r="E22" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A22="","",C22*D22)</f>
         <v>318</v>
       </c>
       <c r="F22" s="18"/>
@@ -1339,7 +1377,7 @@
       <c r="A23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="22">
         <v>43398</v>
       </c>
       <c r="C23" s="3">
@@ -1349,7 +1387,7 @@
         <v>80.33</v>
       </c>
       <c r="E23" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A23="","",C23*D23)</f>
         <v>321.32</v>
       </c>
       <c r="F23" s="18"/>
@@ -1372,7 +1410,7 @@
         <v>9.85</v>
       </c>
       <c r="E24" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A24="","",C24*D24)</f>
         <v>295.5</v>
       </c>
       <c r="F24" s="18"/>
@@ -1394,7 +1432,7 @@
         <v>10.050000000000001</v>
       </c>
       <c r="E25" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A25="","",C25*D25)</f>
         <v>60.300000000000004</v>
       </c>
       <c r="F25" s="18"/>
@@ -1416,7 +1454,7 @@
         <v>101.05</v>
       </c>
       <c r="E26" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A26="","",C26*D26)</f>
         <v>707.35</v>
       </c>
       <c r="F26" s="18"/>
@@ -1438,7 +1476,7 @@
         <v>10.07</v>
       </c>
       <c r="E27" s="14">
-        <f t="shared" si="0"/>
+        <f>IF(A27="","",C27*D27)</f>
         <v>302.10000000000002</v>
       </c>
       <c r="F27" s="18"/>
@@ -1478,7 +1516,7 @@
         <v>105.15</v>
       </c>
       <c r="P28" s="14">
-        <f>IF(L28="","",N28*O28)</f>
+        <f t="shared" ref="P28:P56" si="0">IF(L28="","",N28*O28)</f>
         <v>630.90000000000009</v>
       </c>
       <c r="U28" s="18"/>
@@ -1515,7 +1553,7 @@
         <v>105.1</v>
       </c>
       <c r="P29" s="14">
-        <f>IF(L29="","",N29*O29)</f>
+        <f t="shared" si="0"/>
         <v>945.9</v>
       </c>
       <c r="U29" s="18"/>
@@ -1552,7 +1590,7 @@
         <v>105</v>
       </c>
       <c r="P30" s="14">
-        <f>IF(L30="","",N30*O30)</f>
+        <f t="shared" si="0"/>
         <v>525</v>
       </c>
       <c r="U30" s="18"/>
@@ -1589,7 +1627,7 @@
         <v>105.65</v>
       </c>
       <c r="P31" s="14">
-        <f>IF(L31="","",N31*O31)</f>
+        <f t="shared" si="0"/>
         <v>950.85</v>
       </c>
       <c r="U31" s="18"/>
@@ -1626,7 +1664,7 @@
         <v>105.63</v>
       </c>
       <c r="P32" s="14">
-        <f>IF(L32="","",N32*O32)</f>
+        <f t="shared" si="0"/>
         <v>1056.3</v>
       </c>
       <c r="U32" s="18"/>
@@ -1663,7 +1701,7 @@
         <v>104.5</v>
       </c>
       <c r="P33" s="14">
-        <f>IF(L33="","",N33*O33)</f>
+        <f t="shared" si="0"/>
         <v>1045</v>
       </c>
       <c r="U33" s="18"/>
@@ -1703,7 +1741,7 @@
         <v>116.7</v>
       </c>
       <c r="P34" s="14">
-        <f>IF(L34="","",N34*O34)</f>
+        <f t="shared" si="0"/>
         <v>933.6</v>
       </c>
       <c r="U34" s="18"/>
@@ -1740,7 +1778,7 @@
         <v>105.55</v>
       </c>
       <c r="P35" s="14">
-        <f>IF(L35="","",N35*O35)</f>
+        <f t="shared" si="0"/>
         <v>633.29999999999995</v>
       </c>
       <c r="U35" s="18"/>
@@ -1777,7 +1815,7 @@
         <v>107.9</v>
       </c>
       <c r="P36" s="14">
-        <f>IF(L36="","",N36*O36)</f>
+        <f t="shared" si="0"/>
         <v>647.40000000000009</v>
       </c>
       <c r="U36" s="18"/>
@@ -1814,7 +1852,7 @@
         <v>104.45</v>
       </c>
       <c r="P37" s="14">
-        <f>IF(L37="","",N37*O37)</f>
+        <f t="shared" si="0"/>
         <v>626.70000000000005</v>
       </c>
       <c r="U37" s="18"/>
@@ -1851,7 +1889,7 @@
         <v>107.85</v>
       </c>
       <c r="P38" s="14">
-        <f>IF(L38="","",N38*O38)</f>
+        <f t="shared" si="0"/>
         <v>647.09999999999991</v>
       </c>
       <c r="U38" s="18"/>
@@ -1888,7 +1926,7 @@
         <v>104.59</v>
       </c>
       <c r="P39" s="14">
-        <f>IF(L39="","",N39*O39)</f>
+        <f t="shared" si="0"/>
         <v>627.54</v>
       </c>
       <c r="U39" s="18"/>
@@ -1925,7 +1963,7 @@
         <v>110.57</v>
       </c>
       <c r="P40" s="14">
-        <f>IF(L40="","",N40*O40)</f>
+        <f t="shared" si="0"/>
         <v>1105.6999999999998</v>
       </c>
       <c r="U40" s="18"/>
@@ -1961,7 +1999,7 @@
         <v>106.5</v>
       </c>
       <c r="P41" s="27">
-        <f>IF(L41="","",N41*O41)</f>
+        <f t="shared" si="0"/>
         <v>852</v>
       </c>
       <c r="U41" s="32"/>
@@ -1998,7 +2036,7 @@
         <v>107.65</v>
       </c>
       <c r="P42" s="14">
-        <f>IF(L42="","",N42*O42)</f>
+        <f t="shared" si="0"/>
         <v>322.95000000000005</v>
       </c>
       <c r="U42" s="18"/>
@@ -2038,7 +2076,7 @@
         <v>101</v>
       </c>
       <c r="P43" s="14">
-        <f>IF(L43="","",N43*O43)</f>
+        <f t="shared" si="0"/>
         <v>1313</v>
       </c>
       <c r="U43" s="18"/>
@@ -2078,7 +2116,7 @@
         <v>10.51</v>
       </c>
       <c r="P44" s="14">
-        <f>IF(L44="","",N44*O44)</f>
+        <f t="shared" si="0"/>
         <v>231.22</v>
       </c>
       <c r="U44" s="18"/>
@@ -2115,7 +2153,7 @@
         <v>107.41</v>
       </c>
       <c r="P45" s="14">
-        <f>IF(L45="","",N45*O45)</f>
+        <f t="shared" si="0"/>
         <v>644.46</v>
       </c>
       <c r="U45" s="18"/>
@@ -2152,7 +2190,7 @@
         <v>106.34</v>
       </c>
       <c r="P46" s="14">
-        <f>IF(L46="","",N46*O46)</f>
+        <f t="shared" si="0"/>
         <v>1063.4000000000001</v>
       </c>
       <c r="U46" s="18"/>
@@ -2189,7 +2227,7 @@
         <v>107.35</v>
       </c>
       <c r="P47" s="14">
-        <f>IF(L47="","",N47*O47)</f>
+        <f t="shared" si="0"/>
         <v>214.7</v>
       </c>
       <c r="U47" s="18"/>
@@ -2226,7 +2264,7 @@
         <v>106.68</v>
       </c>
       <c r="P48" s="14">
-        <f>IF(L48="","",N48*O48)</f>
+        <f t="shared" si="0"/>
         <v>106.68</v>
       </c>
       <c r="U48" s="18"/>
@@ -2236,15 +2274,12 @@
       <c r="B49" s="25"/>
       <c r="C49" s="25"/>
       <c r="D49" s="24"/>
-      <c r="E49" s="24" t="str">
-        <f>IF(A49="","",C49*D49)</f>
-        <v/>
-      </c>
+      <c r="E49" s="24"/>
       <c r="F49" s="25"/>
       <c r="K49" s="18"/>
       <c r="O49" s="14"/>
       <c r="P49" s="14" t="str">
-        <f>IF(L49="","",N49*O49)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="U49" s="18"/>
@@ -2254,7 +2289,7 @@
       <c r="K50" s="18"/>
       <c r="O50" s="14"/>
       <c r="P50" s="14" t="str">
-        <f>IF(L50="","",N50*O50)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="U50" s="18"/>
@@ -2263,7 +2298,7 @@
       <c r="F51" s="18"/>
       <c r="K51" s="18"/>
       <c r="P51" s="14" t="str">
-        <f>IF(L51="","",N51*O51)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="U51" s="18"/>
@@ -2272,7 +2307,7 @@
       <c r="F52" s="18"/>
       <c r="K52" s="18"/>
       <c r="P52" s="14" t="str">
-        <f>IF(L52="","",N52*O52)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="U52" s="18"/>
@@ -2281,7 +2316,7 @@
       <c r="F53" s="18"/>
       <c r="K53" s="18"/>
       <c r="P53" s="14" t="str">
-        <f>IF(L53="","",N53*O53)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="U53" s="18"/>
@@ -2290,7 +2325,7 @@
       <c r="F54" s="18"/>
       <c r="K54" s="18"/>
       <c r="P54" s="14" t="str">
-        <f>IF(L54="","",N54*O54)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="U54" s="18"/>
@@ -2299,7 +2334,7 @@
       <c r="F55" s="18"/>
       <c r="K55" s="18"/>
       <c r="P55" s="14" t="str">
-        <f>IF(L55="","",N55*O55)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="U55" s="18"/>
@@ -2308,16 +2343,13 @@
       <c r="F56" s="18"/>
       <c r="K56" s="18"/>
       <c r="P56" s="14" t="str">
-        <f>IF(L56="","",N56*O56)</f>
-        <v/>
-      </c>
-      <c r="U56" s="18"/>
-    </row>
-    <row r="57" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="E57" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="U56" s="18"/>
+    </row>
+    <row r="57" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="E57" s="14"/>
       <c r="F57" s="18"/>
       <c r="K57" s="18"/>
       <c r="P57" s="18"/>
@@ -7909,8 +7941,1317 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F695A9BB-F595-4E34-8FA9-17B0E218AAE9}">
+  <sheetPr codeName="Planilha2"/>
+  <dimension ref="A1:E76"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="29">
+        <v>43504</v>
+      </c>
+      <c r="C2" s="36">
+        <v>15</v>
+      </c>
+      <c r="D2" s="37">
+        <v>0.88</v>
+      </c>
+      <c r="E2" s="37">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="29">
+        <v>43509</v>
+      </c>
+      <c r="C3" s="36">
+        <v>8</v>
+      </c>
+      <c r="D3" s="37">
+        <v>0.46</v>
+      </c>
+      <c r="E3" s="37">
+        <v>3.68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="29">
+        <v>43510</v>
+      </c>
+      <c r="C4" s="36">
+        <v>19</v>
+      </c>
+      <c r="D4" s="37">
+        <v>0.60368421052631582</v>
+      </c>
+      <c r="E4" s="37">
+        <v>11.47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="29">
+        <v>43510</v>
+      </c>
+      <c r="C5" s="36">
+        <v>5</v>
+      </c>
+      <c r="D5" s="37">
+        <v>0.74</v>
+      </c>
+      <c r="E5" s="37">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="29">
+        <v>43510</v>
+      </c>
+      <c r="C6" s="36">
+        <v>8</v>
+      </c>
+      <c r="D6" s="37">
+        <v>0.48</v>
+      </c>
+      <c r="E6" s="37">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="29">
+        <v>43510</v>
+      </c>
+      <c r="C7" s="36">
+        <v>88</v>
+      </c>
+      <c r="D7" s="37">
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="E7" s="37">
+        <v>5.28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="29">
+        <v>43511</v>
+      </c>
+      <c r="C8" s="36">
+        <v>7</v>
+      </c>
+      <c r="D8" s="37">
+        <v>1</v>
+      </c>
+      <c r="E8" s="37">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="29">
+        <v>43511</v>
+      </c>
+      <c r="C9" s="36">
+        <v>4</v>
+      </c>
+      <c r="D9" s="37">
+        <v>1.02</v>
+      </c>
+      <c r="E9" s="37">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="29">
+        <v>43514</v>
+      </c>
+      <c r="C10" s="36">
+        <v>22</v>
+      </c>
+      <c r="D10" s="37">
+        <v>0.51909090909090905</v>
+      </c>
+      <c r="E10" s="37">
+        <v>11.42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="29">
+        <v>43517</v>
+      </c>
+      <c r="C11" s="36">
+        <v>19</v>
+      </c>
+      <c r="D11" s="37">
+        <v>0.62947368421052641</v>
+      </c>
+      <c r="E11" s="37">
+        <v>11.96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="29">
+        <v>43517</v>
+      </c>
+      <c r="C12" s="36">
+        <v>10</v>
+      </c>
+      <c r="D12" s="37">
+        <v>0.6</v>
+      </c>
+      <c r="E12" s="37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="29">
+        <v>43523</v>
+      </c>
+      <c r="C13" s="36">
+        <v>100</v>
+      </c>
+      <c r="D13" s="37">
+        <v>0.68229999999999991</v>
+      </c>
+      <c r="E13" s="37">
+        <v>68.22999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="29">
+        <v>43536</v>
+      </c>
+      <c r="C14" s="36">
+        <v>23</v>
+      </c>
+      <c r="D14" s="37">
+        <v>0.57782608695652171</v>
+      </c>
+      <c r="E14" s="37">
+        <v>13.29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="29">
+        <v>43539</v>
+      </c>
+      <c r="C15" s="36">
+        <v>7</v>
+      </c>
+      <c r="D15" s="37">
+        <v>0.88</v>
+      </c>
+      <c r="E15" s="37">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="29">
+        <v>43539</v>
+      </c>
+      <c r="C16" s="36">
+        <v>8</v>
+      </c>
+      <c r="D16" s="37">
+        <v>0.63</v>
+      </c>
+      <c r="E16" s="37">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="29">
+        <v>43539</v>
+      </c>
+      <c r="C17" s="36">
+        <v>88</v>
+      </c>
+      <c r="D17" s="37">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E17" s="37">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="29">
+        <v>43539</v>
+      </c>
+      <c r="C18" s="36">
+        <v>4</v>
+      </c>
+      <c r="D18" s="37">
+        <v>0.99</v>
+      </c>
+      <c r="E18" s="37">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="29">
+        <v>43542</v>
+      </c>
+      <c r="C19" s="36">
+        <v>19</v>
+      </c>
+      <c r="D19" s="37">
+        <v>0.60368421052631582</v>
+      </c>
+      <c r="E19" s="37">
+        <v>11.47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="29">
+        <v>43542</v>
+      </c>
+      <c r="C20" s="36">
+        <v>8</v>
+      </c>
+      <c r="D20" s="37">
+        <v>0.48</v>
+      </c>
+      <c r="E20" s="37">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="29">
+        <v>43542</v>
+      </c>
+      <c r="C21" s="36">
+        <v>5</v>
+      </c>
+      <c r="D21" s="37">
+        <v>0.6</v>
+      </c>
+      <c r="E21" s="37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="29">
+        <v>43544</v>
+      </c>
+      <c r="C22" s="36">
+        <v>22</v>
+      </c>
+      <c r="D22" s="37">
+        <v>0.65</v>
+      </c>
+      <c r="E22" s="37">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="29">
+        <v>43549</v>
+      </c>
+      <c r="C23" s="36">
+        <v>19</v>
+      </c>
+      <c r="D23" s="37">
+        <v>0.6</v>
+      </c>
+      <c r="E23" s="37">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="29">
+        <v>43550</v>
+      </c>
+      <c r="C24" s="36">
+        <v>10</v>
+      </c>
+      <c r="D24" s="37">
+        <v>0.6</v>
+      </c>
+      <c r="E24" s="37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="29">
+        <v>43580</v>
+      </c>
+      <c r="C25" s="36">
+        <v>10</v>
+      </c>
+      <c r="D25" s="37">
+        <v>0.54</v>
+      </c>
+      <c r="E25" s="37">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="29">
+        <v>43563</v>
+      </c>
+      <c r="C26" s="36">
+        <v>8</v>
+      </c>
+      <c r="D26" s="37">
+        <v>0.17</v>
+      </c>
+      <c r="E26" s="37">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="29">
+        <v>43563</v>
+      </c>
+      <c r="C27" s="36">
+        <v>23</v>
+      </c>
+      <c r="D27" s="37">
+        <v>0.51</v>
+      </c>
+      <c r="E27" s="37">
+        <v>11.73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="29">
+        <v>43563</v>
+      </c>
+      <c r="C28" s="36">
+        <v>15</v>
+      </c>
+      <c r="D28" s="37">
+        <v>0.16999999999999998</v>
+      </c>
+      <c r="E28" s="37">
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="29">
+        <v>43566</v>
+      </c>
+      <c r="C29" s="36">
+        <v>8</v>
+      </c>
+      <c r="D29" s="37">
+        <v>0.81</v>
+      </c>
+      <c r="E29" s="37">
+        <v>6.48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="29">
+        <v>43567</v>
+      </c>
+      <c r="C30" s="36">
+        <v>5</v>
+      </c>
+      <c r="D30" s="37">
+        <v>0.6</v>
+      </c>
+      <c r="E30" s="37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="29">
+        <v>43567</v>
+      </c>
+      <c r="C31" s="36">
+        <v>8</v>
+      </c>
+      <c r="D31" s="37">
+        <v>0.48</v>
+      </c>
+      <c r="E31" s="37">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="29">
+        <v>43567</v>
+      </c>
+      <c r="C32" s="36">
+        <v>19</v>
+      </c>
+      <c r="D32" s="37">
+        <v>0.60368421052631582</v>
+      </c>
+      <c r="E32" s="37">
+        <v>11.47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="29">
+        <v>43570</v>
+      </c>
+      <c r="C33" s="36">
+        <v>4</v>
+      </c>
+      <c r="D33" s="37">
+        <v>0.94</v>
+      </c>
+      <c r="E33" s="37">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="29">
+        <v>43570</v>
+      </c>
+      <c r="C34" s="36">
+        <v>88</v>
+      </c>
+      <c r="D34" s="37">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E34" s="37">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="29">
+        <v>43570</v>
+      </c>
+      <c r="C35" s="36">
+        <v>7</v>
+      </c>
+      <c r="D35" s="37">
+        <v>0.92</v>
+      </c>
+      <c r="E35" s="37">
+        <v>6.44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="29">
+        <v>43571</v>
+      </c>
+      <c r="C36" s="36">
+        <v>22</v>
+      </c>
+      <c r="D36" s="37">
+        <v>0.65</v>
+      </c>
+      <c r="E36" s="37">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="29">
+        <v>43580</v>
+      </c>
+      <c r="C37" s="36">
+        <v>19</v>
+      </c>
+      <c r="D37" s="37">
+        <v>0.54</v>
+      </c>
+      <c r="E37" s="37">
+        <v>10.26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="29">
+        <v>43567</v>
+      </c>
+      <c r="C38" s="36">
+        <v>6</v>
+      </c>
+      <c r="D38" s="37">
+        <v>0.6</v>
+      </c>
+      <c r="E38" s="37">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="29">
+        <v>43567</v>
+      </c>
+      <c r="C39" s="36">
+        <v>10</v>
+      </c>
+      <c r="D39" s="37">
+        <v>0.74</v>
+      </c>
+      <c r="E39" s="37">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="29">
+        <v>43571</v>
+      </c>
+      <c r="C40" s="36">
+        <v>18</v>
+      </c>
+      <c r="D40" s="37">
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="E40" s="37">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="29">
+        <v>43580</v>
+      </c>
+      <c r="C41" s="36">
+        <v>6</v>
+      </c>
+      <c r="D41" s="37">
+        <v>0.54</v>
+      </c>
+      <c r="E41" s="37">
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="29">
+        <v>43609</v>
+      </c>
+      <c r="C42" s="36">
+        <v>10</v>
+      </c>
+      <c r="D42" s="37">
+        <v>0.51</v>
+      </c>
+      <c r="E42" s="37">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="29">
+        <v>43594</v>
+      </c>
+      <c r="C43" s="36">
+        <v>23</v>
+      </c>
+      <c r="D43" s="37">
+        <v>0.67</v>
+      </c>
+      <c r="E43" s="37">
+        <v>15.41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="29">
+        <v>43599</v>
+      </c>
+      <c r="C44" s="36">
+        <v>8</v>
+      </c>
+      <c r="D44" s="37">
+        <v>0.85</v>
+      </c>
+      <c r="E44" s="37">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="29">
+        <v>43600</v>
+      </c>
+      <c r="C45" s="36">
+        <v>4</v>
+      </c>
+      <c r="D45" s="37">
+        <v>1.08</v>
+      </c>
+      <c r="E45" s="37">
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="29">
+        <v>43600</v>
+      </c>
+      <c r="C46" s="36">
+        <v>19</v>
+      </c>
+      <c r="D46" s="37">
+        <v>0.49000000000000005</v>
+      </c>
+      <c r="E46" s="37">
+        <v>9.31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="29">
+        <v>43600</v>
+      </c>
+      <c r="C47" s="36">
+        <v>8</v>
+      </c>
+      <c r="D47" s="37">
+        <v>0.49</v>
+      </c>
+      <c r="E47" s="37">
+        <v>3.92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="29">
+        <v>43600</v>
+      </c>
+      <c r="C48" s="36">
+        <v>22</v>
+      </c>
+      <c r="D48" s="37">
+        <v>0.01</v>
+      </c>
+      <c r="E48" s="37">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="29">
+        <v>43600</v>
+      </c>
+      <c r="C49" s="36">
+        <v>88</v>
+      </c>
+      <c r="D49" s="37">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E49" s="37">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="29">
+        <v>43600</v>
+      </c>
+      <c r="C50" s="36">
+        <v>5</v>
+      </c>
+      <c r="D50" s="37">
+        <v>0.6</v>
+      </c>
+      <c r="E50" s="37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="29">
+        <v>43600</v>
+      </c>
+      <c r="C51" s="36">
+        <v>7</v>
+      </c>
+      <c r="D51" s="37">
+        <v>0.91</v>
+      </c>
+      <c r="E51" s="37">
+        <v>6.37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="29">
+        <v>43602</v>
+      </c>
+      <c r="C52" s="36">
+        <v>22</v>
+      </c>
+      <c r="D52" s="37">
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="E52" s="37">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="29">
+        <v>43602</v>
+      </c>
+      <c r="C53" s="36">
+        <v>13</v>
+      </c>
+      <c r="D53" s="37">
+        <v>0.3923076923076923</v>
+      </c>
+      <c r="E53" s="37">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="29">
+        <v>43609</v>
+      </c>
+      <c r="C54" s="36">
+        <v>19</v>
+      </c>
+      <c r="D54" s="37">
+        <v>0.51</v>
+      </c>
+      <c r="E54" s="37">
+        <v>9.69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A55" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="29">
+        <v>43600</v>
+      </c>
+      <c r="C55" s="36">
+        <v>10</v>
+      </c>
+      <c r="D55" s="37">
+        <v>0.74</v>
+      </c>
+      <c r="E55" s="37">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A56" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="29">
+        <v>43600</v>
+      </c>
+      <c r="C56" s="36">
+        <v>17</v>
+      </c>
+      <c r="D56" s="37">
+        <v>0.6</v>
+      </c>
+      <c r="E56" s="37">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A57" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="29">
+        <v>43600</v>
+      </c>
+      <c r="C57" s="36">
+        <v>9</v>
+      </c>
+      <c r="D57" s="37">
+        <v>0.49</v>
+      </c>
+      <c r="E57" s="37">
+        <v>4.41</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A58" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="29">
+        <v>43602</v>
+      </c>
+      <c r="C58" s="36">
+        <v>18</v>
+      </c>
+      <c r="D58" s="37">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E58" s="37">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A59" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" s="29">
+        <v>43607</v>
+      </c>
+      <c r="C59" s="36">
+        <v>200</v>
+      </c>
+      <c r="D59" s="37">
+        <v>0.33340000000000003</v>
+      </c>
+      <c r="E59" s="37">
+        <v>66.680000000000007</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A60" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" s="29">
+        <v>43630</v>
+      </c>
+      <c r="C60" s="36">
+        <v>10</v>
+      </c>
+      <c r="D60" s="37">
+        <v>0.74</v>
+      </c>
+      <c r="E60" s="37">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A61" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="29">
+        <v>43630</v>
+      </c>
+      <c r="C61" s="36">
+        <v>36</v>
+      </c>
+      <c r="D61" s="37">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="E61" s="37">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A62" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" s="29">
+        <v>43630</v>
+      </c>
+      <c r="C62" s="36">
+        <v>9</v>
+      </c>
+      <c r="D62" s="37">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E62" s="37">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A63" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" s="29">
+        <v>43634</v>
+      </c>
+      <c r="C63" s="36">
+        <v>47</v>
+      </c>
+      <c r="D63" s="37">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E63" s="37">
+        <v>25.85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A64" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="29">
+        <v>43626</v>
+      </c>
+      <c r="C64" s="36">
+        <v>23</v>
+      </c>
+      <c r="D64" s="37">
+        <v>0.72</v>
+      </c>
+      <c r="E64" s="37">
+        <v>16.559999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A65" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" s="29">
+        <v>43629</v>
+      </c>
+      <c r="C65" s="36">
+        <v>8</v>
+      </c>
+      <c r="D65" s="37">
+        <v>0.85</v>
+      </c>
+      <c r="E65" s="37">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A66" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="29">
+        <v>43630</v>
+      </c>
+      <c r="C66" s="36">
+        <v>7</v>
+      </c>
+      <c r="D66" s="37">
+        <v>0.96</v>
+      </c>
+      <c r="E66" s="37">
+        <v>6.72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A67" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67" s="29">
+        <v>43630</v>
+      </c>
+      <c r="C67" s="36">
+        <v>5</v>
+      </c>
+      <c r="D67" s="37">
+        <v>0.6</v>
+      </c>
+      <c r="E67" s="37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A68" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" s="29">
+        <v>43630</v>
+      </c>
+      <c r="C68" s="36">
+        <v>110</v>
+      </c>
+      <c r="D68" s="37">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E68" s="37">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A69" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="29">
+        <v>43630</v>
+      </c>
+      <c r="C69" s="36">
+        <v>8</v>
+      </c>
+      <c r="D69" s="37">
+        <v>0.49</v>
+      </c>
+      <c r="E69" s="37">
+        <v>3.92</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" s="29">
+        <v>43630</v>
+      </c>
+      <c r="C70" s="36">
+        <v>19</v>
+      </c>
+      <c r="D70" s="37">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E70" s="37">
+        <v>10.64</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A71" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71" s="29">
+        <v>43630</v>
+      </c>
+      <c r="C71" s="36">
+        <v>4</v>
+      </c>
+      <c r="D71" s="37">
+        <v>1.05</v>
+      </c>
+      <c r="E71" s="37">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A72" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72" s="29">
+        <v>43634</v>
+      </c>
+      <c r="C72" s="36">
+        <v>35</v>
+      </c>
+      <c r="D72" s="37">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E72" s="37">
+        <v>19.25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A73" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73" s="29">
+        <v>43641</v>
+      </c>
+      <c r="C73" s="36">
+        <v>10</v>
+      </c>
+      <c r="D73" s="37">
+        <v>0.54</v>
+      </c>
+      <c r="E73" s="37">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A74" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" s="29">
+        <v>43641</v>
+      </c>
+      <c r="C74" s="36">
+        <v>19</v>
+      </c>
+      <c r="D74" s="37">
+        <v>0.54</v>
+      </c>
+      <c r="E74" s="36">
+        <v>10.26</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A75" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B75" s="29">
+        <v>43641</v>
+      </c>
+      <c r="C75" s="36">
+        <v>39</v>
+      </c>
+      <c r="D75" s="37">
+        <v>0.6594871794871795</v>
+      </c>
+      <c r="E75" s="36">
+        <v>25.72</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A76" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" s="29">
+        <v>43641</v>
+      </c>
+      <c r="C76" s="36">
+        <v>32</v>
+      </c>
+      <c r="D76" s="37">
+        <v>0.54</v>
+      </c>
+      <c r="E76" s="36">
+        <v>17.28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Planilha3">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:X995"/>

</xml_diff>